<commit_message>
Updated evidence spreadsheet for github.
</commit_message>
<xml_diff>
--- a/docs/Evidence/Attachment E Approach Criteria Evidence Template Mod 5.xlsx
+++ b/docs/Evidence/Attachment E Approach Criteria Evidence Template Mod 5.xlsx
@@ -144,143 +144,121 @@
     <t>q</t>
   </si>
   <si>
+    <t>We setup and used Zabbix to perform continuous monitoring of our development/test environment and our production environment.
+Digital Playbook#12 Use data to drive decisions
+URL: 
+http://medexplorer.northropgrumman.com:9001/zabbix/dashboard.php</t>
+  </si>
+  <si>
     <t>We assigned our Product Manager (Ray R.) and gave him the authority, responsibility, and accountability for the MedExplorer prototype. 
 Digital Playbook# 6 Assign one leader and hold that person accountable
 URL: 
-http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/MedExplorer%20Development%20Team.md</t>
+http://github.com/NorthropGrumman/MedExplorer/blob/master/docs/MedExplorer%20Development%20Team.md</t>
   </si>
   <si>
     <t>Our MedExplorer development team used 10 of the labor categories to design and develop the prototype. 
 Digital Playbook#7 Bring in experienced teams
 URL:
-http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/MedExplorer%20Development%20Team.md</t>
+http://github.com/NorthropGrumman/MedExplorer/blob/master/docs/MedExplorer%20Development%20Team.md</t>
   </si>
   <si>
     <t>Our User Experience design team interviewed and performed user tests with a number for General Public and Clinician users. The team also met with Northrop Grumman's Clinical Advisory Group as part of our Health Division. Users participated in periodic demonstrations for feedback. Created scenarios and stories. The team gave periodic demonstrations to walk through scenarios and gather feedback. We captured feedback as user stories and added to the backlog for prioritization.
 Digital Playbook#1: Understand what people need
 URL: 
-http://git.triad.local/NorthropGrumman/MedExplorer/tree/master/docs/User%20Centered%20Design/Research%20Findings
-http://git.triad.local/NorthropGrumman/MedExplorer/tree/master/docs/User%20Centered%20Design/Scenarios
-http://git.triad.local/NorthropGrumman/MedExplorer/tree/master/docs/Software%20Development/User-Stories</t>
+http://github.com/NorthropGrumman/MedExplorer/tree/master/docs/User%20Centered%20Design/Research%20Findings
+http://github.com/NorthropGrumman/MedExplorer/tree/master/docs/User%20Centered%20Design/Scenarios
+http://github.com/NorthropGrumman/MedExplorer/tree/master/docs/Software%20Development/User-Stories</t>
   </si>
   <si>
     <t>Our User Centered Design approach used a number of techniques and tools, including interviews, focus groups, expectancy tests, generative research, and usability tests.
 Digital Playbook#3 Make it simple and intuitive
 URL: 
-http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/User%20Centered%20Design/Readme.md</t>
+http://github.com/NorthropGrumman/MedExplorer/blob/master/docs/User%20Centered%20Design/Readme.md</t>
   </si>
   <si>
     <t>Our UX team created a design style guide to provide guidance for the web front end developers. Style guides were updated each sprint with development.
 Digital Playbook#3 Make it simple and intuitive
 URL: 
-http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/User%20Centered%20Design/Design%20Style%20Guide/Style_Guide_Master.pdf</t>
+http://github.com/NorthropGrumman/MedExplorer/blob/master/docs/User%20Centered%20Design/Design%20Style%20Guide/Style_Guide_Master.pdf</t>
   </si>
   <si>
     <t>Our UX team performed a number of usability tests with users and provided feedback to the development staff.
 Once we had some initial features in place, usability tests were run daily.
 Digital Playbook#4 Build the service using agile and iterative practices
 URL: 
-http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/User%20Centered%20Design/Research%20Findings/Focus%20Group2.pdf
-http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/User%20Centered%20Design/Research%20Findings/Generative_Research.pdf</t>
+http://github.com/NorthropGrumman/MedExplorer/blob/master/docs/User%20Centered%20Design/Research%20Findings/Focus%20Group2.pdf
+http://github.com/NorthropGrumman/MedExplorer/blob/master/docs/User%20Centered%20Design/Research%20Findings/Generative_Research.pdf</t>
   </si>
   <si>
     <t>Using our Agile framework, which is built upon Scrum, Extreme Programming, and user-centered design techniques, we were able to develop the product in an iterative fashion while receiving regular, timely feedback from users and stakeholders. We conducted an initial sprint 0 as we identified the team and coordinated the infrastructure. Then we used sprint cycles of 5 hours each comprised of sprint planning, execution, and review (demo and retrospective).
 Digital Playbook#4 Build the service using agile and iterative practices
 URL: 
-http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/Software%20Development/Processes/Readme.md
-http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/User%20Centered%20Design/Readme.md
-http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/Software%20Development/Iterative%20Development.md
-http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/User%20Centered%20Design/Research%20Findings/Generative_Research.pdf</t>
+http://github.com/NorthropGrumman/MedExplorer/blob/master/docs/Software%20Development/Processes/Readme.md
+http://github.com/NorthropGrumman/MedExplorer/blob/master/docs/User%20Centered%20Design/Readme.md
+http://github.com/NorthropGrumman/MedExplorer/blob/master/docs/Software%20Development/Iterative%20Development.md
+http://github.com/NorthropGrumman/MedExplorer/blob/master/docs/User%20Centered%20Design/Research%20Findings/Generative_Research.pdf</t>
   </si>
   <si>
     <t>Our MedExplorer prototype was design for multiple platforms including PCs, laptops, tablets, and phones.
 Digital Playbook#2 Address the whole experience, from start to finish
 Digital Playbook#7 Bring in experienced teams
 URL: 
-http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/Software%20Development/Platform%20Support.md</t>
+http://github.com/NorthropGrumman/MedExplorer/blob/master/docs/Software%20Development/Platform%20Support.md</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Our MedExplorer used a number of modern, open source technologies, including TwitterBootstrap, AngularJS, NodeJS, ExpressJS, Docker, MongoDB, Jenkins and Zabbix.
+Digital Playbook#8 Choose a modern technology stack
+URL: 
+http://github.com/NorthropGrumman/MedExplorer/blob/master/License.md#open-source-third-party-software-licenses
+http://github.com/NorthropGrumman/MedExplorer/blob/master/docs/Diagrams/MedExplorer_TechnologyStack.png
+</t>
   </si>
   <si>
     <t xml:space="preserve">Our MedExplorer prototype is deployed on a IaaS provider, we selected IBM SoftLayers as our provider.
 Digital Playbook#9 Deploy in a flexible hosting environment
 URL: 
 http://MedExplorer.northropgrumman.com
-http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/Software%20Development/Screenshots/softlayer.png
+http://github.com/NorthropGrumman/MedExplorer/blob/master/docs/Software%20Development/Screenshots/softlayer.png
 </t>
   </si>
   <si>
     <t>Our development wrote unit tests for their code and was part of the team's definition of done. The front-end unit testing is done using the Jasmine testing framework, which is run by the Karma test-runner. The back-end code is tested using the UnitJS testing framework and is run by mocha. These unit tests were automated using Jenkins so that they run after every commit. 
 Digital Playbook#10 Automate testing and deployments
 URL: 
-http://git.triad.local/NorthropGrumman/MedExplorer/tree/master/src/client/test 
-http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/Pictures/Definition%20of%20Done.jpg
-http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/Software%20Development/Processes/DevOps.md#unit-testing-and-automated-test</t>
+http://github.com/NorthropGrumman/MedExplorer/tree/master/src/client/test 
+http://github.com/NorthropGrumman/MedExplorer/blob/master/docs/Pictures/Definition%20of%20Done.jpg
+http://github.com/NorthropGrumman/MedExplorer/blob/master/docs/Software%20Development/Processes/DevOps.md#unit-testing-and-automated-test</t>
   </si>
   <si>
     <t>Our development team used Jenkins for our continuous integration system to automate running of tests and to perform continuous deployment.
 Digital Playbook#10 Automate testing and deployments
 URL: 
-http://git.triad.local/NorthropGrumman/MedExplorer/tree/master/docs/Software%20Development/Screenshots#jenkins
-http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/Software%20Development/Processes/DevOps.md#continuous-integration</t>
+http://github.com/NorthropGrumman/MedExplorer/tree/master/docs/Software%20Development/Screenshots#jenkins
+http://github.com/NorthropGrumman/MedExplorer/blob/master/docs/Software%20Development/Processes/DevOps.md#continuous-integration</t>
   </si>
   <si>
-    <t>We setup and used Zabbix to perform continuous monitoring of our development/test environment and our production environment.
-Digital Playbook#12 Use data to drive decisions
+    <t>We used an internal GitHub Enterprise server as our configuration management systems.
+Digital Playbook#4 Build the service using agile and iterative practices
 URL: 
-http://medexplorer.northropgrumman.com:9001/zabbix/dashboard.php</t>
+http://github.com/NorthropGrumman/MedExplorer/tree/master/docs/Software%20Development/Screenshots#github</t>
   </si>
   <si>
     <t>We used Docker as our container system for our MedExplorer prototype.
 Digital Playbook#4 Build the service using agile and iterative practices
 Digital Playbook#9 Deploy in a flexible hosting environment
-http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/Software%20Development/Processes/DevOps.md#continuous-deliverydeployment</t>
+http://github.com/NorthropGrumman/MedExplorer/blob/master/docs/Software%20Development/Processes/DevOps.md#continuous-deliverydeployment</t>
   </si>
   <si>
     <t>We have provided instructions for installing MedExplorer in your own Docker container system.
 Digital Playbook#9 Deploy in a flexible hosting environment
 URL: 
-http://git.triad.local/NorthropGrumman/MedExplorer/tree/master/docs/Install%20Procedures</t>
+http://github.com/NorthropGrumman/MedExplorer/tree/master/docs/Install%20Procedures</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">We used an internal GitHub Enterprise server as our </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>configuration management systems.
-Digital Playbook#4 Build the service using agile and iterative practices
+    <t>The MedExplorer prototype and underlying platforms, components, and frameworks used on the project were open source licensed and free of charge.
+Digital Playbook#13 Default to open
 URL: 
-http://git.triad.local/NorthropGrumman/MedExplorer/tree/master/docs/Software%20Development/Screenshots#github</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The MedExplorer prototype and underlying platforms, components, and frameworks used on the project were open source licensed and free of charge.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Digital Playbook#13 Default to open
-URL: 
-http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/License.md</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Our MedExplorer used a number of modern, open source technologies, including TwitterBootstrap, AngularJS, NodeJS, ExpressJS, Docker, MongoDB, Jenkins and Zabbix.
-Digital Playbook#8 Choose a modern technology stack
-URL: 
-http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/License.md#open-source-third-party-software-licenses
-http://git.triad.local/NorthropGrumman/MedExplorer/blob/master/docs/Diagrams/MedExplorer_TechnologyStack.png
-</t>
+http://github.com/NorthropGrumman/MedExplorer/blob/master/License.md</t>
   </si>
 </sst>
 </file>
@@ -10938,7 +10916,7 @@
   <dimension ref="A1:F998"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10972,7 +10950,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -10986,7 +10964,7 @@
         <v>22</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -11000,7 +10978,7 @@
         <v>25</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -11014,7 +10992,7 @@
         <v>27</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -11028,7 +11006,7 @@
         <v>31</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -11042,7 +11020,7 @@
         <v>33</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -11056,7 +11034,7 @@
         <v>23</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -11070,7 +11048,7 @@
         <v>34</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -11084,7 +11062,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -11098,7 +11076,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -11112,7 +11090,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -11126,7 +11104,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -11140,7 +11118,7 @@
         <v>16</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -11154,7 +11132,7 @@
         <v>18</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -11168,7 +11146,7 @@
         <v>20</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -11182,7 +11160,7 @@
         <v>26</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -11196,7 +11174,7 @@
         <v>30</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>

</xml_diff>